<commit_message>
Added Date in the UI along with time, now date will be chosen based on the present dat3!
</commit_message>
<xml_diff>
--- a/productivity_log.xlsx
+++ b/productivity_log.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>Date</t>
+  </si>
   <si>
     <t>Time Period</t>
   </si>
@@ -25,22 +28,16 @@
     <t>Win/Lost</t>
   </si>
   <si>
-    <t>22-23</t>
-  </si>
-  <si>
-    <t>8-9</t>
-  </si>
-  <si>
-    <t>GoodndksfaskldZ</t>
-  </si>
-  <si>
-    <t>hiiiiiii</t>
-  </si>
-  <si>
-    <t>Win</t>
-  </si>
-  <si>
-    <t>Lost</t>
+    <t>2024-08-30</t>
+  </si>
+  <si>
+    <t>3-4</t>
+  </si>
+  <si>
+    <t>cdsf</t>
+  </si>
+  <si>
+    <t>fsdf</t>
   </si>
 </sst>
 </file>
@@ -398,13 +395,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -414,27 +411,22 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Paths as Dropdown, For making the process of choosing the paths easier!
</commit_message>
<xml_diff>
--- a/productivity_log.xlsx
+++ b/productivity_log.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -34,10 +34,19 @@
     <t>3-4</t>
   </si>
   <si>
+    <t>2-3</t>
+  </si>
+  <si>
     <t>cdsf</t>
   </si>
   <si>
+    <t>hitdujgrfjdthgfdsfgf</t>
+  </si>
+  <si>
     <t>fsdf</t>
+  </si>
+  <si>
+    <t>Win</t>
   </si>
 </sst>
 </file>
@@ -395,7 +404,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -423,10 +432,24 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made win/lost column as points column where i can enter how much points i earned in that particular hour- the target will be always to win 5 points
</commit_message>
<xml_diff>
--- a/productivity_log.xlsx
+++ b/productivity_log.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20413"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kamalesh.kb\KAMALESH_PRODUCTIVITY\Productivity\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF4EE56-03F9-46DD-9F7A-5F0A55759024}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -31,29 +37,41 @@
     <t>2024-08-30</t>
   </si>
   <si>
-    <t>3-4</t>
+    <t>11-12</t>
+  </si>
+  <si>
+    <t>12-13</t>
+  </si>
+  <si>
+    <t>13-14</t>
   </si>
   <si>
     <t>2-3</t>
   </si>
   <si>
-    <t>cdsf</t>
-  </si>
-  <si>
-    <t>hitdujgrfjdthgfdsfgf</t>
-  </si>
-  <si>
-    <t>fsdf</t>
-  </si>
-  <si>
-    <t>Win</t>
+    <t>15-16</t>
+  </si>
+  <si>
+    <t>Made code for cleaning the influx data(for Supriya)</t>
+  </si>
+  <si>
+    <t>Not too good(as didn't got the output for automatic anomaly removal)</t>
+  </si>
+  <si>
+    <t>Lunch Time- Discussions during the lunch time went healthy,1.40- 2.00 to finish the lunch!More concentration need to be given .</t>
+  </si>
+  <si>
+    <t>Taught Srijanani how to visualise the CAN DBC and the twai transmit code.</t>
+  </si>
+  <si>
+    <t>Not able to concentrate on the essentials as the disturbance was too much present on the lab premises</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,17 +123,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -162,7 +189,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -194,9 +221,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -228,6 +273,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -403,14 +466,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="106.88671875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -424,7 +492,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -432,13 +500,13 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -446,10 +514,52 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
-        <v>10</v>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>